<commit_message>
czech tooltip for awards
</commit_message>
<xml_diff>
--- a/7. Návody pro ocenění/Medajle.xlsx
+++ b/7. Návody pro ocenění/Medajle.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20399"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="20401"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lpesek\Documents\Projekty\BattleField2Ranks\7. Návody pro ocenění\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\lpesek\Documents\Final Projects\BFHQ\7. Návody pro ocenění\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B43FEBEC-FD98-4CD6-A1D2-D8764FDA9EC0}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{92165CF9-C50C-4E71-B5E4-A89641F8F54B}" xr6:coauthVersionLast="36" xr6:coauthVersionMax="36" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="25200" windowHeight="12036" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -223,9 +223,6 @@
     <t>kills3</t>
   </si>
   <si>
-    <t>Celkově 100 hodin jako velitel týmů</t>
-  </si>
-  <si>
     <t>Celkově 100 hodin jako tým leader</t>
   </si>
   <si>
@@ -265,9 +262,6 @@
     <t>24 zabití v jednom kole</t>
   </si>
   <si>
-    <t>NESMÍTE ZABÍT ANI ZRANIT SPOLUHRÁČE V TOMTO KOLE (ani poškodit vozidlo</t>
-  </si>
-  <si>
     <t>time</t>
   </si>
   <si>
@@ -404,6 +398,12 @@
   </si>
   <si>
     <t xml:space="preserve">Medajle za zvláštní službu Evropské unie </t>
+  </si>
+  <si>
+    <t>Celkově 100 hodin jako velitel týmu</t>
+  </si>
+  <si>
+    <t>NESMÍTE ZABÍT ANI ZRANIT SPOLUHRÁČE V TOMTO KOLE (ani poškodit vozidlo)</t>
   </si>
 </sst>
 </file>
@@ -688,122 +688,122 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="1" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="3" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="3" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="center" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -2048,8 +2048,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H74"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
-      <selection activeCell="C16" sqref="C16:C18"/>
+    <sheetView tabSelected="1" topLeftCell="A15" zoomScale="205" zoomScaleNormal="205" workbookViewId="0">
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.109375" defaultRowHeight="9.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -2066,42 +2066,42 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="19"/>
-      <c r="B1" s="19" t="s">
+      <c r="A1" s="55"/>
+      <c r="B1" s="55" t="s">
         <v>0</v>
       </c>
-      <c r="C1" s="17" t="s">
+      <c r="C1" s="54" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="19" t="s">
+      <c r="D1" s="55" t="s">
         <v>2</v>
       </c>
-      <c r="E1" s="19"/>
-      <c r="F1" s="19"/>
-      <c r="G1" s="19"/>
-      <c r="H1" s="17" t="s">
+      <c r="E1" s="55"/>
+      <c r="F1" s="55"/>
+      <c r="G1" s="55"/>
+      <c r="H1" s="54" t="s">
         <v>7</v>
       </c>
     </row>
     <row r="2" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A2" s="19"/>
-      <c r="B2" s="19"/>
-      <c r="C2" s="17"/>
-      <c r="D2" s="17" t="s">
+      <c r="A2" s="55"/>
+      <c r="B2" s="55"/>
+      <c r="C2" s="54"/>
+      <c r="D2" s="54" t="s">
         <v>3</v>
       </c>
-      <c r="E2" s="19" t="s">
+      <c r="E2" s="55" t="s">
         <v>4</v>
       </c>
-      <c r="F2" s="19"/>
-      <c r="G2" s="19"/>
-      <c r="H2" s="17"/>
+      <c r="F2" s="55"/>
+      <c r="G2" s="55"/>
+      <c r="H2" s="54"/>
     </row>
     <row r="3" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A3" s="19"/>
-      <c r="B3" s="19"/>
-      <c r="C3" s="17"/>
-      <c r="D3" s="17"/>
+      <c r="A3" s="55"/>
+      <c r="B3" s="55"/>
+      <c r="C3" s="54"/>
+      <c r="D3" s="54"/>
       <c r="E3" s="5" t="s">
         <v>5</v>
       </c>
@@ -2111,149 +2111,149 @@
       <c r="G3" s="5" t="s">
         <v>8</v>
       </c>
-      <c r="H3" s="17"/>
+      <c r="H3" s="54"/>
     </row>
     <row r="4" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A4" s="21">
+      <c r="A4" s="26">
         <v>1</v>
       </c>
-      <c r="B4" s="18"/>
-      <c r="C4" s="20" t="s">
+      <c r="B4" s="31"/>
+      <c r="C4" s="32" t="s">
         <v>9</v>
       </c>
-      <c r="D4" s="20" t="s">
+      <c r="D4" s="32" t="s">
         <v>13</v>
       </c>
-      <c r="E4" s="18" t="s">
+      <c r="E4" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F4" s="18" t="s">
+      <c r="F4" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="G4" s="20" t="s">
+      <c r="G4" s="32" t="s">
         <v>21</v>
       </c>
-      <c r="H4" s="18">
+      <c r="H4" s="31">
         <v>2051902</v>
       </c>
     </row>
     <row r="5" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A5" s="21"/>
-      <c r="B5" s="18"/>
-      <c r="C5" s="20"/>
-      <c r="D5" s="20"/>
-      <c r="E5" s="18"/>
-      <c r="F5" s="18"/>
-      <c r="G5" s="20"/>
-      <c r="H5" s="18"/>
+      <c r="A5" s="26"/>
+      <c r="B5" s="31"/>
+      <c r="C5" s="32"/>
+      <c r="D5" s="32"/>
+      <c r="E5" s="31"/>
+      <c r="F5" s="31"/>
+      <c r="G5" s="32"/>
+      <c r="H5" s="31"/>
     </row>
     <row r="6" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A6" s="21"/>
-      <c r="B6" s="18"/>
-      <c r="C6" s="20"/>
-      <c r="D6" s="20"/>
-      <c r="E6" s="18"/>
-      <c r="F6" s="18"/>
-      <c r="G6" s="20"/>
-      <c r="H6" s="18"/>
+      <c r="A6" s="26"/>
+      <c r="B6" s="31"/>
+      <c r="C6" s="32"/>
+      <c r="D6" s="32"/>
+      <c r="E6" s="31"/>
+      <c r="F6" s="31"/>
+      <c r="G6" s="32"/>
+      <c r="H6" s="31"/>
     </row>
     <row r="7" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A7" s="21">
+      <c r="A7" s="26">
         <v>2</v>
       </c>
-      <c r="B7" s="22"/>
-      <c r="C7" s="23" t="s">
+      <c r="B7" s="25"/>
+      <c r="C7" s="27" t="s">
         <v>10</v>
       </c>
-      <c r="D7" s="23" t="s">
+      <c r="D7" s="27" t="s">
         <v>14</v>
       </c>
-      <c r="E7" s="22" t="s">
+      <c r="E7" s="25" t="s">
         <v>17</v>
       </c>
-      <c r="F7" s="22" t="s">
+      <c r="F7" s="25" t="s">
         <v>20</v>
       </c>
-      <c r="G7" s="23" t="s">
+      <c r="G7" s="27" t="s">
         <v>22</v>
       </c>
-      <c r="H7" s="22">
+      <c r="H7" s="25">
         <v>2051919</v>
       </c>
     </row>
     <row r="8" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A8" s="21"/>
-      <c r="B8" s="22"/>
-      <c r="C8" s="23"/>
-      <c r="D8" s="23"/>
-      <c r="E8" s="22"/>
-      <c r="F8" s="22"/>
-      <c r="G8" s="23"/>
-      <c r="H8" s="22"/>
+      <c r="A8" s="26"/>
+      <c r="B8" s="25"/>
+      <c r="C8" s="27"/>
+      <c r="D8" s="27"/>
+      <c r="E8" s="25"/>
+      <c r="F8" s="25"/>
+      <c r="G8" s="27"/>
+      <c r="H8" s="25"/>
     </row>
     <row r="9" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A9" s="21"/>
-      <c r="B9" s="22"/>
-      <c r="C9" s="23"/>
-      <c r="D9" s="23"/>
-      <c r="E9" s="22"/>
-      <c r="F9" s="22"/>
-      <c r="G9" s="23"/>
-      <c r="H9" s="22"/>
+      <c r="A9" s="26"/>
+      <c r="B9" s="25"/>
+      <c r="C9" s="27"/>
+      <c r="D9" s="27"/>
+      <c r="E9" s="25"/>
+      <c r="F9" s="25"/>
+      <c r="G9" s="27"/>
+      <c r="H9" s="25"/>
     </row>
     <row r="10" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A10" s="21">
+      <c r="A10" s="26">
         <v>3</v>
       </c>
-      <c r="B10" s="18"/>
-      <c r="C10" s="20" t="s">
+      <c r="B10" s="31"/>
+      <c r="C10" s="32" t="s">
         <v>11</v>
       </c>
-      <c r="D10" s="20" t="s">
+      <c r="D10" s="32" t="s">
         <v>15</v>
       </c>
-      <c r="E10" s="18" t="s">
+      <c r="E10" s="31" t="s">
         <v>17</v>
       </c>
-      <c r="F10" s="18" t="s">
+      <c r="F10" s="31" t="s">
         <v>20</v>
       </c>
-      <c r="G10" s="20" t="s">
+      <c r="G10" s="32" t="s">
         <v>23</v>
       </c>
-      <c r="H10" s="18">
+      <c r="H10" s="31">
         <v>2051907</v>
       </c>
     </row>
     <row r="11" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A11" s="21"/>
-      <c r="B11" s="18"/>
-      <c r="C11" s="20"/>
-      <c r="D11" s="20"/>
-      <c r="E11" s="18"/>
-      <c r="F11" s="18"/>
-      <c r="G11" s="20"/>
-      <c r="H11" s="18"/>
+      <c r="A11" s="26"/>
+      <c r="B11" s="31"/>
+      <c r="C11" s="32"/>
+      <c r="D11" s="32"/>
+      <c r="E11" s="31"/>
+      <c r="F11" s="31"/>
+      <c r="G11" s="32"/>
+      <c r="H11" s="31"/>
     </row>
     <row r="12" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A12" s="21"/>
-      <c r="B12" s="18"/>
-      <c r="C12" s="20"/>
-      <c r="D12" s="20"/>
-      <c r="E12" s="18"/>
-      <c r="F12" s="18"/>
-      <c r="G12" s="20"/>
-      <c r="H12" s="18"/>
+      <c r="A12" s="26"/>
+      <c r="B12" s="31"/>
+      <c r="C12" s="32"/>
+      <c r="D12" s="32"/>
+      <c r="E12" s="31"/>
+      <c r="F12" s="31"/>
+      <c r="G12" s="32"/>
+      <c r="H12" s="31"/>
     </row>
     <row r="13" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A13" s="21">
+      <c r="A13" s="26">
         <v>4</v>
       </c>
-      <c r="B13" s="22"/>
-      <c r="C13" s="23" t="s">
+      <c r="B13" s="25"/>
+      <c r="C13" s="27" t="s">
         <v>12</v>
       </c>
-      <c r="D13" s="23" t="s">
+      <c r="D13" s="27" t="s">
         <v>16</v>
       </c>
       <c r="E13" s="7" t="s">
@@ -2265,42 +2265,42 @@
       <c r="G13" s="7">
         <v>5</v>
       </c>
-      <c r="H13" s="22">
+      <c r="H13" s="25">
         <v>2191608</v>
       </c>
     </row>
     <row r="14" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A14" s="21"/>
-      <c r="B14" s="22"/>
-      <c r="C14" s="23"/>
-      <c r="D14" s="23"/>
-      <c r="E14" s="26" t="s">
+      <c r="A14" s="26"/>
+      <c r="B14" s="25"/>
+      <c r="C14" s="27"/>
+      <c r="D14" s="27"/>
+      <c r="E14" s="23" t="s">
         <v>17</v>
       </c>
-      <c r="F14" s="26" t="s">
+      <c r="F14" s="23" t="s">
         <v>19</v>
       </c>
-      <c r="G14" s="26">
+      <c r="G14" s="23">
         <v>20</v>
       </c>
-      <c r="H14" s="22"/>
+      <c r="H14" s="25"/>
     </row>
     <row r="15" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A15" s="21"/>
-      <c r="B15" s="22"/>
-      <c r="C15" s="23"/>
-      <c r="D15" s="23"/>
-      <c r="E15" s="27"/>
-      <c r="F15" s="27"/>
-      <c r="G15" s="27"/>
-      <c r="H15" s="22"/>
+      <c r="A15" s="26"/>
+      <c r="B15" s="25"/>
+      <c r="C15" s="27"/>
+      <c r="D15" s="27"/>
+      <c r="E15" s="53"/>
+      <c r="F15" s="53"/>
+      <c r="G15" s="53"/>
+      <c r="H15" s="25"/>
     </row>
     <row r="16" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="21">
+      <c r="A16" s="26">
         <v>5</v>
       </c>
-      <c r="B16" s="18"/>
-      <c r="C16" s="20" t="s">
+      <c r="B16" s="31"/>
+      <c r="C16" s="32" t="s">
         <v>24</v>
       </c>
       <c r="D16" s="9" t="s">
@@ -2315,14 +2315,14 @@
       <c r="G16" s="6">
         <v>360000</v>
       </c>
-      <c r="H16" s="18">
+      <c r="H16" s="31">
         <v>2021403</v>
       </c>
     </row>
     <row r="17" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A17" s="21"/>
-      <c r="B17" s="18"/>
-      <c r="C17" s="20"/>
+      <c r="A17" s="26"/>
+      <c r="B17" s="31"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="9" t="s">
         <v>27</v>
       </c>
@@ -2335,12 +2335,12 @@
       <c r="G17" s="6">
         <v>100</v>
       </c>
-      <c r="H17" s="18"/>
+      <c r="H17" s="31"/>
     </row>
     <row r="18" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A18" s="21"/>
-      <c r="B18" s="18"/>
-      <c r="C18" s="20"/>
+      <c r="A18" s="26"/>
+      <c r="B18" s="31"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="9" t="s">
         <v>41</v>
       </c>
@@ -2353,46 +2353,46 @@
       <c r="G18" s="6">
         <v>100</v>
       </c>
-      <c r="H18" s="18"/>
+      <c r="H18" s="31"/>
     </row>
     <row r="19" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="21">
+      <c r="A19" s="26">
         <v>6</v>
       </c>
-      <c r="B19" s="22"/>
-      <c r="C19" s="23" t="s">
+      <c r="B19" s="25"/>
+      <c r="C19" s="27" t="s">
         <v>25</v>
       </c>
-      <c r="D19" s="24" t="s">
+      <c r="D19" s="17" t="s">
         <v>33</v>
       </c>
-      <c r="E19" s="26" t="s">
+      <c r="E19" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F19" s="26" t="s">
+      <c r="F19" s="23" t="s">
         <v>34</v>
       </c>
-      <c r="G19" s="26">
+      <c r="G19" s="23">
         <v>360000</v>
       </c>
-      <c r="H19" s="22">
+      <c r="H19" s="25">
         <v>2020719</v>
       </c>
     </row>
     <row r="20" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A20" s="21"/>
-      <c r="B20" s="22"/>
-      <c r="C20" s="23"/>
-      <c r="D20" s="25"/>
-      <c r="E20" s="27"/>
-      <c r="F20" s="27"/>
-      <c r="G20" s="27"/>
-      <c r="H20" s="22"/>
+      <c r="A20" s="26"/>
+      <c r="B20" s="25"/>
+      <c r="C20" s="27"/>
+      <c r="D20" s="52"/>
+      <c r="E20" s="53"/>
+      <c r="F20" s="53"/>
+      <c r="G20" s="53"/>
+      <c r="H20" s="25"/>
     </row>
     <row r="21" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="21"/>
-      <c r="B21" s="22"/>
-      <c r="C21" s="23"/>
+      <c r="A21" s="26"/>
+      <c r="B21" s="25"/>
+      <c r="C21" s="27"/>
       <c r="D21" s="8" t="s">
         <v>32</v>
       </c>
@@ -2405,42 +2405,42 @@
       <c r="G21" s="7">
         <v>100</v>
       </c>
-      <c r="H21" s="22"/>
+      <c r="H21" s="25"/>
     </row>
     <row r="22" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A22" s="21"/>
-      <c r="B22" s="22"/>
-      <c r="C22" s="23"/>
-      <c r="D22" s="24" t="s">
+      <c r="A22" s="26"/>
+      <c r="B22" s="25"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="17" t="s">
         <v>40</v>
       </c>
-      <c r="E22" s="26" t="s">
+      <c r="E22" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="F22" s="26" t="s">
+      <c r="F22" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="G22" s="26">
+      <c r="G22" s="23">
         <v>100</v>
       </c>
-      <c r="H22" s="22"/>
+      <c r="H22" s="25"/>
     </row>
     <row r="23" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A23" s="21"/>
-      <c r="B23" s="22"/>
-      <c r="C23" s="23"/>
-      <c r="D23" s="25"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="22"/>
+      <c r="A23" s="26"/>
+      <c r="B23" s="25"/>
+      <c r="C23" s="27"/>
+      <c r="D23" s="52"/>
+      <c r="E23" s="53"/>
+      <c r="F23" s="53"/>
+      <c r="G23" s="53"/>
+      <c r="H23" s="25"/>
     </row>
     <row r="24" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="21">
+      <c r="A24" s="26">
         <v>7</v>
       </c>
-      <c r="B24" s="18"/>
-      <c r="C24" s="20" t="s">
+      <c r="B24" s="31"/>
+      <c r="C24" s="32" t="s">
         <v>46</v>
       </c>
       <c r="D24" s="9" t="s">
@@ -2455,14 +2455,14 @@
       <c r="G24" s="6">
         <v>360000</v>
       </c>
-      <c r="H24" s="18">
+      <c r="H24" s="31">
         <v>2021613</v>
       </c>
     </row>
     <row r="25" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="21"/>
-      <c r="B25" s="18"/>
-      <c r="C25" s="20"/>
+      <c r="A25" s="26"/>
+      <c r="B25" s="31"/>
+      <c r="C25" s="32"/>
       <c r="D25" s="9" t="s">
         <v>38</v>
       </c>
@@ -2475,12 +2475,12 @@
       <c r="G25" s="6">
         <v>100</v>
       </c>
-      <c r="H25" s="18"/>
+      <c r="H25" s="31"/>
     </row>
     <row r="26" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="21"/>
-      <c r="B26" s="18"/>
-      <c r="C26" s="20"/>
+      <c r="A26" s="26"/>
+      <c r="B26" s="31"/>
+      <c r="C26" s="32"/>
       <c r="D26" s="9" t="s">
         <v>39</v>
       </c>
@@ -2493,74 +2493,74 @@
       <c r="G26" s="6">
         <v>100</v>
       </c>
-      <c r="H26" s="18"/>
+      <c r="H26" s="31"/>
     </row>
     <row r="27" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A27" s="45">
+      <c r="A27" s="19">
         <v>8</v>
       </c>
-      <c r="B27" s="47"/>
-      <c r="C27" s="24" t="s">
-        <v>124</v>
+      <c r="B27" s="21"/>
+      <c r="C27" s="17" t="s">
+        <v>122</v>
       </c>
       <c r="D27" s="12" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="E27" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F27" s="11" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="G27" s="11">
         <v>180000</v>
       </c>
-      <c r="H27" s="26">
+      <c r="H27" s="23">
         <v>3270519</v>
       </c>
     </row>
     <row r="28" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A28" s="46"/>
-      <c r="B28" s="48"/>
-      <c r="C28" s="44"/>
+      <c r="A28" s="20"/>
+      <c r="B28" s="22"/>
+      <c r="C28" s="18"/>
       <c r="D28" s="12" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="E28" s="11" t="s">
         <v>28</v>
       </c>
       <c r="F28" s="11" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="G28" s="11">
         <v>100</v>
       </c>
-      <c r="H28" s="49"/>
+      <c r="H28" s="24"/>
     </row>
     <row r="29" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="46"/>
-      <c r="B29" s="48"/>
-      <c r="C29" s="44"/>
+      <c r="A29" s="20"/>
+      <c r="B29" s="22"/>
+      <c r="C29" s="18"/>
       <c r="D29" s="14" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="E29" s="15" t="s">
         <v>28</v>
       </c>
       <c r="F29" s="15" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="G29" s="15">
         <v>100</v>
       </c>
-      <c r="H29" s="49"/>
+      <c r="H29" s="24"/>
     </row>
     <row r="30" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="21">
+      <c r="A30" s="26">
         <v>9</v>
       </c>
-      <c r="B30" s="18"/>
-      <c r="C30" s="20" t="s">
+      <c r="B30" s="31"/>
+      <c r="C30" s="32" t="s">
         <v>45</v>
       </c>
       <c r="D30" s="13" t="s">
@@ -2575,14 +2575,14 @@
       <c r="G30" s="10">
         <v>360000</v>
       </c>
-      <c r="H30" s="18">
+      <c r="H30" s="31">
         <v>2190318</v>
       </c>
     </row>
     <row r="31" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A31" s="21"/>
-      <c r="B31" s="18"/>
-      <c r="C31" s="20"/>
+      <c r="A31" s="26"/>
+      <c r="B31" s="31"/>
+      <c r="C31" s="32"/>
       <c r="D31" s="13" t="s">
         <v>50</v>
       </c>
@@ -2595,12 +2595,12 @@
       <c r="G31" s="10">
         <v>5000</v>
       </c>
-      <c r="H31" s="18"/>
+      <c r="H31" s="31"/>
     </row>
     <row r="32" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A32" s="21"/>
-      <c r="B32" s="18"/>
-      <c r="C32" s="20"/>
+      <c r="A32" s="26"/>
+      <c r="B32" s="31"/>
+      <c r="C32" s="32"/>
       <c r="D32" s="13" t="s">
         <v>52</v>
       </c>
@@ -2613,14 +2613,14 @@
       <c r="G32" s="10">
         <v>25</v>
       </c>
-      <c r="H32" s="18"/>
+      <c r="H32" s="31"/>
     </row>
     <row r="33" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="21">
+      <c r="A33" s="26">
         <v>10</v>
       </c>
-      <c r="B33" s="22"/>
-      <c r="C33" s="23" t="s">
+      <c r="B33" s="25"/>
+      <c r="C33" s="27" t="s">
         <v>47</v>
       </c>
       <c r="D33" s="12" t="s">
@@ -2635,14 +2635,14 @@
       <c r="G33" s="11">
         <v>360000</v>
       </c>
-      <c r="H33" s="22">
+      <c r="H33" s="25">
         <v>2190309</v>
       </c>
     </row>
     <row r="34" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A34" s="21"/>
-      <c r="B34" s="22"/>
-      <c r="C34" s="23"/>
+      <c r="A34" s="26"/>
+      <c r="B34" s="25"/>
+      <c r="C34" s="27"/>
       <c r="D34" s="12" t="s">
         <v>56</v>
       </c>
@@ -2655,12 +2655,12 @@
       <c r="G34" s="11">
         <v>5000</v>
       </c>
-      <c r="H34" s="22"/>
+      <c r="H34" s="25"/>
     </row>
     <row r="35" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A35" s="21"/>
-      <c r="B35" s="22"/>
-      <c r="C35" s="23"/>
+      <c r="A35" s="26"/>
+      <c r="B35" s="25"/>
+      <c r="C35" s="27"/>
       <c r="D35" s="12" t="s">
         <v>57</v>
       </c>
@@ -2673,14 +2673,14 @@
       <c r="G35" s="11">
         <v>25</v>
       </c>
-      <c r="H35" s="22"/>
+      <c r="H35" s="25"/>
     </row>
     <row r="36" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A36" s="21">
+      <c r="A36" s="26">
         <v>11</v>
       </c>
-      <c r="B36" s="18"/>
-      <c r="C36" s="20" t="s">
+      <c r="B36" s="31"/>
+      <c r="C36" s="32" t="s">
         <v>48</v>
       </c>
       <c r="D36" s="13" t="s">
@@ -2695,14 +2695,14 @@
       <c r="G36" s="10">
         <v>360000</v>
       </c>
-      <c r="H36" s="18">
+      <c r="H36" s="31">
         <v>2190308</v>
       </c>
     </row>
     <row r="37" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="21"/>
-      <c r="B37" s="18"/>
-      <c r="C37" s="20"/>
+      <c r="A37" s="26"/>
+      <c r="B37" s="31"/>
+      <c r="C37" s="32"/>
       <c r="D37" s="13" t="s">
         <v>60</v>
       </c>
@@ -2715,12 +2715,12 @@
       <c r="G37" s="10">
         <v>5000</v>
       </c>
-      <c r="H37" s="18"/>
+      <c r="H37" s="31"/>
     </row>
     <row r="38" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A38" s="21"/>
-      <c r="B38" s="18"/>
-      <c r="C38" s="20"/>
+      <c r="A38" s="26"/>
+      <c r="B38" s="31"/>
+      <c r="C38" s="32"/>
       <c r="D38" s="13" t="s">
         <v>61</v>
       </c>
@@ -2733,116 +2733,116 @@
       <c r="G38" s="10">
         <v>25</v>
       </c>
-      <c r="H38" s="18"/>
+      <c r="H38" s="31"/>
     </row>
     <row r="39" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A39" s="21">
+      <c r="A39" s="26">
         <v>12</v>
       </c>
-      <c r="B39" s="22"/>
-      <c r="C39" s="23" t="s">
+      <c r="B39" s="25"/>
+      <c r="C39" s="27" t="s">
         <v>49</v>
       </c>
       <c r="D39" s="12" t="s">
-        <v>64</v>
+        <v>123</v>
       </c>
       <c r="E39" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F39" s="11" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="G39" s="11">
         <v>360000</v>
       </c>
-      <c r="H39" s="22">
+      <c r="H39" s="25">
         <v>2020419</v>
       </c>
     </row>
     <row r="40" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A40" s="21"/>
-      <c r="B40" s="22"/>
-      <c r="C40" s="23"/>
+      <c r="A40" s="26"/>
+      <c r="B40" s="25"/>
+      <c r="C40" s="27"/>
       <c r="D40" s="12" t="s">
-        <v>65</v>
+        <v>64</v>
       </c>
       <c r="E40" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F40" s="11" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="G40" s="11">
         <v>360000</v>
       </c>
-      <c r="H40" s="22"/>
+      <c r="H40" s="25"/>
     </row>
     <row r="41" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A41" s="21"/>
-      <c r="B41" s="22"/>
-      <c r="C41" s="23"/>
+      <c r="A41" s="26"/>
+      <c r="B41" s="25"/>
+      <c r="C41" s="27"/>
       <c r="D41" s="12" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="E41" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F41" s="11" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="G41" s="11">
         <v>360000</v>
       </c>
-      <c r="H41" s="22"/>
+      <c r="H41" s="25"/>
     </row>
     <row r="42" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A42" s="21"/>
-      <c r="B42" s="22"/>
-      <c r="C42" s="23"/>
+      <c r="A42" s="26"/>
+      <c r="B42" s="25"/>
+      <c r="C42" s="27"/>
       <c r="D42" s="12" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="E42" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F42" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G42" s="11">
         <v>45</v>
       </c>
-      <c r="H42" s="22"/>
+      <c r="H42" s="25"/>
     </row>
     <row r="43" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A43" s="21">
+      <c r="A43" s="26">
         <v>13</v>
       </c>
-      <c r="B43" s="18"/>
-      <c r="C43" s="20" t="s">
-        <v>72</v>
+      <c r="B43" s="31"/>
+      <c r="C43" s="32" t="s">
+        <v>71</v>
       </c>
       <c r="D43" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E43" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F43" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G43" s="10">
         <v>900000</v>
       </c>
-      <c r="H43" s="18">
+      <c r="H43" s="31">
         <v>2190703</v>
       </c>
     </row>
     <row r="44" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A44" s="21"/>
-      <c r="B44" s="18"/>
-      <c r="C44" s="20"/>
+      <c r="A44" s="26"/>
+      <c r="B44" s="31"/>
+      <c r="C44" s="32"/>
       <c r="D44" s="13" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="E44" s="10" t="s">
         <v>17</v>
@@ -2853,66 +2853,66 @@
       <c r="G44" s="10">
         <v>24</v>
       </c>
-      <c r="H44" s="18"/>
+      <c r="H44" s="31"/>
     </row>
     <row r="45" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A45" s="21"/>
-      <c r="B45" s="18"/>
-      <c r="C45" s="20"/>
-      <c r="D45" s="30" t="s">
+      <c r="A45" s="26"/>
+      <c r="B45" s="31"/>
+      <c r="C45" s="32"/>
+      <c r="D45" s="50" t="s">
+        <v>124</v>
+      </c>
+      <c r="E45" s="48" t="s">
+        <v>17</v>
+      </c>
+      <c r="F45" s="48" t="s">
         <v>78</v>
       </c>
-      <c r="E45" s="28" t="s">
-        <v>17</v>
-      </c>
-      <c r="F45" s="28" t="s">
-        <v>80</v>
-      </c>
-      <c r="G45" s="28">
+      <c r="G45" s="48">
         <v>0</v>
       </c>
-      <c r="H45" s="18"/>
+      <c r="H45" s="31"/>
     </row>
     <row r="46" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A46" s="21"/>
-      <c r="B46" s="18"/>
-      <c r="C46" s="20"/>
-      <c r="D46" s="31"/>
-      <c r="E46" s="29"/>
-      <c r="F46" s="29"/>
-      <c r="G46" s="29"/>
-      <c r="H46" s="18"/>
+      <c r="A46" s="26"/>
+      <c r="B46" s="31"/>
+      <c r="C46" s="32"/>
+      <c r="D46" s="51"/>
+      <c r="E46" s="49"/>
+      <c r="F46" s="49"/>
+      <c r="G46" s="49"/>
+      <c r="H46" s="31"/>
     </row>
     <row r="47" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A47" s="21">
+      <c r="A47" s="26">
         <v>14</v>
       </c>
-      <c r="B47" s="22"/>
-      <c r="C47" s="23" t="s">
-        <v>73</v>
+      <c r="B47" s="25"/>
+      <c r="C47" s="27" t="s">
+        <v>72</v>
       </c>
       <c r="D47" s="12" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E47" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F47" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G47" s="11">
         <v>900000</v>
       </c>
-      <c r="H47" s="22">
+      <c r="H47" s="25">
         <v>2190303</v>
       </c>
     </row>
     <row r="48" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A48" s="21"/>
-      <c r="B48" s="22"/>
-      <c r="C48" s="23"/>
+      <c r="A48" s="26"/>
+      <c r="B48" s="25"/>
+      <c r="C48" s="27"/>
       <c r="D48" s="12" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="E48" s="11" t="s">
         <v>17</v>
@@ -2923,428 +2923,520 @@
       <c r="G48" s="11">
         <v>25000</v>
       </c>
-      <c r="H48" s="22"/>
+      <c r="H48" s="25"/>
     </row>
     <row r="49" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A49" s="21"/>
-      <c r="B49" s="22"/>
-      <c r="C49" s="23"/>
+      <c r="A49" s="26"/>
+      <c r="B49" s="25"/>
+      <c r="C49" s="27"/>
       <c r="D49" s="12" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="E49" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F49" s="11" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="G49" s="11">
         <v>25</v>
       </c>
-      <c r="H49" s="22"/>
+      <c r="H49" s="25"/>
     </row>
     <row r="50" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A50" s="21"/>
-      <c r="B50" s="22"/>
-      <c r="C50" s="23"/>
+      <c r="A50" s="26"/>
+      <c r="B50" s="25"/>
+      <c r="C50" s="27"/>
       <c r="D50" s="12" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="E50" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F50" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G50" s="11">
         <v>1980</v>
       </c>
-      <c r="H50" s="22"/>
+      <c r="H50" s="25"/>
     </row>
     <row r="51" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A51" s="21">
+      <c r="A51" s="26">
         <v>15</v>
       </c>
-      <c r="B51" s="18"/>
-      <c r="C51" s="20" t="s">
-        <v>74</v>
+      <c r="B51" s="31"/>
+      <c r="C51" s="32" t="s">
+        <v>73</v>
       </c>
       <c r="D51" s="13" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="E51" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F51" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G51" s="10">
         <v>900000</v>
       </c>
-      <c r="H51" s="18">
+      <c r="H51" s="31">
         <v>2191319</v>
       </c>
     </row>
     <row r="52" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A52" s="21"/>
-      <c r="B52" s="18"/>
-      <c r="C52" s="20"/>
+      <c r="A52" s="26"/>
+      <c r="B52" s="31"/>
+      <c r="C52" s="32"/>
       <c r="D52" s="13" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="E52" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F52" s="10" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="G52" s="10">
         <v>1000</v>
       </c>
-      <c r="H52" s="18"/>
+      <c r="H52" s="31"/>
     </row>
     <row r="53" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A53" s="21"/>
-      <c r="B53" s="18"/>
-      <c r="C53" s="20"/>
+      <c r="A53" s="26"/>
+      <c r="B53" s="31"/>
+      <c r="C53" s="32"/>
       <c r="D53" s="13" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="E53" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F53" s="10" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="G53" s="10">
         <v>1000</v>
       </c>
-      <c r="H53" s="18"/>
+      <c r="H53" s="31"/>
     </row>
     <row r="54" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A54" s="21"/>
-      <c r="B54" s="18"/>
-      <c r="C54" s="20"/>
+      <c r="A54" s="26"/>
+      <c r="B54" s="31"/>
+      <c r="C54" s="32"/>
       <c r="D54" s="13" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="E54" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F54" s="10" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="G54" s="10">
         <v>1000</v>
       </c>
-      <c r="H54" s="18"/>
+      <c r="H54" s="31"/>
     </row>
     <row r="55" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="21"/>
-      <c r="B55" s="18"/>
-      <c r="C55" s="20"/>
-      <c r="D55" s="53" t="s">
-        <v>94</v>
-      </c>
-      <c r="E55" s="54"/>
-      <c r="F55" s="54"/>
-      <c r="G55" s="55"/>
-      <c r="H55" s="18"/>
+      <c r="A55" s="26"/>
+      <c r="B55" s="31"/>
+      <c r="C55" s="32"/>
+      <c r="D55" s="33" t="s">
+        <v>92</v>
+      </c>
+      <c r="E55" s="34"/>
+      <c r="F55" s="34"/>
+      <c r="G55" s="35"/>
+      <c r="H55" s="31"/>
     </row>
     <row r="56" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="21">
+      <c r="A56" s="26">
         <v>16</v>
       </c>
-      <c r="B56" s="22"/>
-      <c r="C56" s="23" t="s">
+      <c r="B56" s="25"/>
+      <c r="C56" s="27" t="s">
+        <v>74</v>
+      </c>
+      <c r="D56" s="12" t="s">
         <v>75</v>
-      </c>
-      <c r="D56" s="12" t="s">
-        <v>76</v>
       </c>
       <c r="E56" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F56" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G56" s="11">
         <v>900000</v>
       </c>
-      <c r="H56" s="22">
+      <c r="H56" s="25">
         <v>2021322</v>
       </c>
     </row>
     <row r="57" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="21"/>
-      <c r="B57" s="22"/>
-      <c r="C57" s="23"/>
+      <c r="A57" s="26"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="27"/>
       <c r="D57" s="12" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="E57" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F57" s="11" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="G57" s="11">
         <v>5000</v>
       </c>
-      <c r="H57" s="22"/>
+      <c r="H57" s="25"/>
     </row>
     <row r="58" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A58" s="21"/>
-      <c r="B58" s="22"/>
-      <c r="C58" s="23"/>
+      <c r="A58" s="26"/>
+      <c r="B58" s="25"/>
+      <c r="C58" s="27"/>
       <c r="D58" s="12" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="E58" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F58" s="11" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="G58" s="11">
         <v>30000</v>
       </c>
-      <c r="H58" s="22"/>
+      <c r="H58" s="25"/>
     </row>
     <row r="59" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A59" s="21"/>
-      <c r="B59" s="22"/>
-      <c r="C59" s="23"/>
+      <c r="A59" s="26"/>
+      <c r="B59" s="25"/>
+      <c r="C59" s="27"/>
       <c r="D59" s="12" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="E59" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F59" s="11" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="G59" s="11">
         <v>1000</v>
       </c>
-      <c r="H59" s="22"/>
+      <c r="H59" s="25"/>
     </row>
     <row r="60" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A60" s="21"/>
-      <c r="B60" s="22"/>
-      <c r="C60" s="23"/>
-      <c r="D60" s="50" t="s">
-        <v>94</v>
-      </c>
-      <c r="E60" s="51"/>
-      <c r="F60" s="51"/>
-      <c r="G60" s="52"/>
-      <c r="H60" s="22"/>
+      <c r="A60" s="26"/>
+      <c r="B60" s="25"/>
+      <c r="C60" s="27"/>
+      <c r="D60" s="28" t="s">
+        <v>92</v>
+      </c>
+      <c r="E60" s="29"/>
+      <c r="F60" s="29"/>
+      <c r="G60" s="30"/>
+      <c r="H60" s="25"/>
     </row>
     <row r="61" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A61" s="21">
+      <c r="A61" s="26">
         <v>17</v>
       </c>
-      <c r="B61" s="18"/>
-      <c r="C61" s="20" t="s">
-        <v>97</v>
+      <c r="B61" s="31"/>
+      <c r="C61" s="32" t="s">
+        <v>95</v>
       </c>
       <c r="D61" s="13" t="s">
-        <v>100</v>
+        <v>98</v>
       </c>
       <c r="E61" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F61" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G61" s="10">
         <v>720000</v>
       </c>
-      <c r="H61" s="18">
+      <c r="H61" s="31">
         <v>2020903</v>
       </c>
     </row>
     <row r="62" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A62" s="21"/>
-      <c r="B62" s="18"/>
-      <c r="C62" s="20"/>
+      <c r="A62" s="26"/>
+      <c r="B62" s="31"/>
+      <c r="C62" s="32"/>
       <c r="D62" s="13" t="s">
+        <v>101</v>
+      </c>
+      <c r="E62" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F62" s="10" t="s">
         <v>103</v>
       </c>
-      <c r="E62" s="10" t="s">
+      <c r="G62" s="10" t="s">
         <v>104</v>
       </c>
-      <c r="F62" s="10" t="s">
-        <v>105</v>
-      </c>
-      <c r="G62" s="10" t="s">
-        <v>106</v>
-      </c>
-      <c r="H62" s="18"/>
+      <c r="H62" s="31"/>
     </row>
     <row r="63" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A63" s="21"/>
-      <c r="B63" s="18"/>
-      <c r="C63" s="20"/>
-      <c r="D63" s="32" t="s">
-        <v>113</v>
-      </c>
-      <c r="E63" s="33"/>
-      <c r="F63" s="33"/>
-      <c r="G63" s="34"/>
-      <c r="H63" s="18"/>
+      <c r="A63" s="26"/>
+      <c r="B63" s="31"/>
+      <c r="C63" s="32"/>
+      <c r="D63" s="36" t="s">
+        <v>111</v>
+      </c>
+      <c r="E63" s="37"/>
+      <c r="F63" s="37"/>
+      <c r="G63" s="38"/>
+      <c r="H63" s="31"/>
     </row>
     <row r="64" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A64" s="21"/>
-      <c r="B64" s="18"/>
-      <c r="C64" s="20"/>
-      <c r="D64" s="35"/>
-      <c r="E64" s="36"/>
-      <c r="F64" s="36"/>
-      <c r="G64" s="37"/>
-      <c r="H64" s="18"/>
+      <c r="A64" s="26"/>
+      <c r="B64" s="31"/>
+      <c r="C64" s="32"/>
+      <c r="D64" s="39"/>
+      <c r="E64" s="40"/>
+      <c r="F64" s="40"/>
+      <c r="G64" s="41"/>
+      <c r="H64" s="31"/>
     </row>
     <row r="65" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A65" s="21">
+      <c r="A65" s="26">
         <v>18</v>
       </c>
-      <c r="B65" s="22"/>
-      <c r="C65" s="23" t="s">
-        <v>98</v>
+      <c r="B65" s="25"/>
+      <c r="C65" s="27" t="s">
+        <v>96</v>
       </c>
       <c r="D65" s="16" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="E65" s="11" t="s">
         <v>17</v>
       </c>
       <c r="F65" s="11" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G65" s="11">
         <v>1080000</v>
       </c>
-      <c r="H65" s="22">
+      <c r="H65" s="25">
         <v>2020913</v>
       </c>
     </row>
     <row r="66" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="21"/>
-      <c r="B66" s="22"/>
-      <c r="C66" s="23"/>
+      <c r="A66" s="26"/>
+      <c r="B66" s="25"/>
+      <c r="C66" s="27"/>
       <c r="D66" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="E66" s="11" t="s">
+        <v>102</v>
+      </c>
+      <c r="F66" s="11" t="s">
+        <v>106</v>
+      </c>
+      <c r="G66" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="E66" s="11" t="s">
-        <v>104</v>
-      </c>
-      <c r="F66" s="11" t="s">
-        <v>108</v>
-      </c>
-      <c r="G66" s="11" t="s">
-        <v>109</v>
-      </c>
-      <c r="H66" s="22"/>
+      <c r="H66" s="25"/>
     </row>
     <row r="67" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="21"/>
-      <c r="B67" s="22"/>
-      <c r="C67" s="23"/>
-      <c r="D67" s="38" t="s">
-        <v>114</v>
-      </c>
-      <c r="E67" s="39"/>
-      <c r="F67" s="39"/>
-      <c r="G67" s="40"/>
-      <c r="H67" s="22"/>
+      <c r="A67" s="26"/>
+      <c r="B67" s="25"/>
+      <c r="C67" s="27"/>
+      <c r="D67" s="42" t="s">
+        <v>112</v>
+      </c>
+      <c r="E67" s="43"/>
+      <c r="F67" s="43"/>
+      <c r="G67" s="44"/>
+      <c r="H67" s="25"/>
     </row>
     <row r="68" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="21"/>
-      <c r="B68" s="22"/>
-      <c r="C68" s="23"/>
-      <c r="D68" s="41"/>
-      <c r="E68" s="42"/>
-      <c r="F68" s="42"/>
-      <c r="G68" s="43"/>
-      <c r="H68" s="22"/>
+      <c r="A68" s="26"/>
+      <c r="B68" s="25"/>
+      <c r="C68" s="27"/>
+      <c r="D68" s="45"/>
+      <c r="E68" s="46"/>
+      <c r="F68" s="46"/>
+      <c r="G68" s="47"/>
+      <c r="H68" s="25"/>
     </row>
     <row r="69" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="21">
+      <c r="A69" s="26">
         <v>19</v>
       </c>
-      <c r="B69" s="18"/>
-      <c r="C69" s="20" t="s">
-        <v>99</v>
+      <c r="B69" s="31"/>
+      <c r="C69" s="32" t="s">
+        <v>97</v>
       </c>
       <c r="D69" s="13" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="E69" s="10" t="s">
         <v>17</v>
       </c>
       <c r="F69" s="10" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="G69" s="10">
         <v>1440000</v>
       </c>
-      <c r="H69" s="18">
+      <c r="H69" s="31">
         <v>2020919</v>
       </c>
     </row>
     <row r="70" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A70" s="21"/>
-      <c r="B70" s="18"/>
-      <c r="C70" s="20"/>
+      <c r="A70" s="26"/>
+      <c r="B70" s="31"/>
+      <c r="C70" s="32"/>
       <c r="D70" s="13" t="s">
+        <v>108</v>
+      </c>
+      <c r="E70" s="10" t="s">
+        <v>102</v>
+      </c>
+      <c r="F70" s="10" t="s">
+        <v>109</v>
+      </c>
+      <c r="G70" s="10" t="s">
         <v>110</v>
       </c>
-      <c r="E70" s="10" t="s">
-        <v>104</v>
-      </c>
-      <c r="F70" s="10" t="s">
-        <v>111</v>
-      </c>
-      <c r="G70" s="10" t="s">
-        <v>112</v>
-      </c>
-      <c r="H70" s="18"/>
+      <c r="H70" s="31"/>
     </row>
     <row r="71" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A71" s="21"/>
-      <c r="B71" s="18"/>
-      <c r="C71" s="20"/>
-      <c r="D71" s="32" t="s">
-        <v>115</v>
-      </c>
-      <c r="E71" s="33"/>
-      <c r="F71" s="33"/>
-      <c r="G71" s="34"/>
-      <c r="H71" s="18"/>
+      <c r="A71" s="26"/>
+      <c r="B71" s="31"/>
+      <c r="C71" s="32"/>
+      <c r="D71" s="36" t="s">
+        <v>113</v>
+      </c>
+      <c r="E71" s="37"/>
+      <c r="F71" s="37"/>
+      <c r="G71" s="38"/>
+      <c r="H71" s="31"/>
     </row>
     <row r="72" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="21"/>
-      <c r="B72" s="18"/>
-      <c r="C72" s="20"/>
-      <c r="D72" s="35"/>
-      <c r="E72" s="36"/>
-      <c r="F72" s="36"/>
-      <c r="G72" s="37"/>
-      <c r="H72" s="18"/>
+      <c r="A72" s="26"/>
+      <c r="B72" s="31"/>
+      <c r="C72" s="32"/>
+      <c r="D72" s="39"/>
+      <c r="E72" s="40"/>
+      <c r="F72" s="40"/>
+      <c r="G72" s="41"/>
+      <c r="H72" s="31"/>
     </row>
     <row r="73" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="1" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
     </row>
     <row r="74" spans="1:8" ht="9.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="1" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="116">
+    <mergeCell ref="A13:A15"/>
+    <mergeCell ref="B13:B15"/>
+    <mergeCell ref="C13:C15"/>
+    <mergeCell ref="D13:D15"/>
+    <mergeCell ref="D22:D23"/>
+    <mergeCell ref="H1:H3"/>
+    <mergeCell ref="H4:H6"/>
+    <mergeCell ref="E2:G2"/>
+    <mergeCell ref="D1:G1"/>
+    <mergeCell ref="G4:G6"/>
+    <mergeCell ref="A1:A3"/>
+    <mergeCell ref="D2:D3"/>
+    <mergeCell ref="C1:C3"/>
+    <mergeCell ref="B1:B3"/>
+    <mergeCell ref="F4:F6"/>
+    <mergeCell ref="E4:E6"/>
+    <mergeCell ref="D4:D6"/>
+    <mergeCell ref="C4:C6"/>
+    <mergeCell ref="B4:B6"/>
+    <mergeCell ref="A4:A6"/>
+    <mergeCell ref="H13:H15"/>
+    <mergeCell ref="A16:A18"/>
+    <mergeCell ref="B16:B18"/>
+    <mergeCell ref="C16:C18"/>
+    <mergeCell ref="H16:H18"/>
+    <mergeCell ref="G14:G15"/>
+    <mergeCell ref="F14:F15"/>
+    <mergeCell ref="E14:E15"/>
+    <mergeCell ref="H7:H9"/>
+    <mergeCell ref="A10:A12"/>
+    <mergeCell ref="B10:B12"/>
+    <mergeCell ref="C10:C12"/>
+    <mergeCell ref="D10:D12"/>
+    <mergeCell ref="E10:E12"/>
+    <mergeCell ref="F10:F12"/>
+    <mergeCell ref="G10:G12"/>
+    <mergeCell ref="H10:H12"/>
+    <mergeCell ref="G7:G9"/>
+    <mergeCell ref="A7:A9"/>
+    <mergeCell ref="B7:B9"/>
+    <mergeCell ref="C7:C9"/>
+    <mergeCell ref="D7:D9"/>
+    <mergeCell ref="E7:E9"/>
+    <mergeCell ref="F7:F9"/>
+    <mergeCell ref="H19:H23"/>
+    <mergeCell ref="A24:A26"/>
+    <mergeCell ref="B24:B26"/>
+    <mergeCell ref="C24:C26"/>
+    <mergeCell ref="A30:A32"/>
+    <mergeCell ref="B30:B32"/>
+    <mergeCell ref="C30:C32"/>
+    <mergeCell ref="H30:H32"/>
+    <mergeCell ref="H24:H26"/>
+    <mergeCell ref="D19:D20"/>
+    <mergeCell ref="E19:E20"/>
+    <mergeCell ref="F19:F20"/>
+    <mergeCell ref="G19:G20"/>
+    <mergeCell ref="G22:G23"/>
+    <mergeCell ref="F22:F23"/>
+    <mergeCell ref="E22:E23"/>
+    <mergeCell ref="A19:A23"/>
+    <mergeCell ref="B19:B23"/>
+    <mergeCell ref="C19:C23"/>
+    <mergeCell ref="C43:C46"/>
+    <mergeCell ref="H43:H46"/>
+    <mergeCell ref="A39:A42"/>
+    <mergeCell ref="G45:G46"/>
+    <mergeCell ref="F45:F46"/>
+    <mergeCell ref="E45:E46"/>
+    <mergeCell ref="D45:D46"/>
+    <mergeCell ref="H33:H35"/>
+    <mergeCell ref="A36:A38"/>
+    <mergeCell ref="B36:B38"/>
+    <mergeCell ref="C36:C38"/>
+    <mergeCell ref="H36:H38"/>
+    <mergeCell ref="A33:A35"/>
+    <mergeCell ref="B33:B35"/>
+    <mergeCell ref="C33:C35"/>
+    <mergeCell ref="A69:A72"/>
+    <mergeCell ref="B69:B72"/>
+    <mergeCell ref="C69:C72"/>
+    <mergeCell ref="H69:H72"/>
+    <mergeCell ref="A65:A68"/>
+    <mergeCell ref="B65:B68"/>
+    <mergeCell ref="C65:C68"/>
+    <mergeCell ref="D63:G64"/>
+    <mergeCell ref="D67:G68"/>
+    <mergeCell ref="D71:G72"/>
+    <mergeCell ref="A61:A64"/>
+    <mergeCell ref="B61:B64"/>
+    <mergeCell ref="C61:C64"/>
+    <mergeCell ref="H61:H64"/>
     <mergeCell ref="C27:C29"/>
     <mergeCell ref="A27:A29"/>
     <mergeCell ref="B27:B29"/>
@@ -3365,102 +3457,10 @@
     <mergeCell ref="H51:H55"/>
     <mergeCell ref="D55:G55"/>
     <mergeCell ref="B39:B42"/>
-    <mergeCell ref="A69:A72"/>
-    <mergeCell ref="B69:B72"/>
-    <mergeCell ref="C69:C72"/>
-    <mergeCell ref="H69:H72"/>
-    <mergeCell ref="A65:A68"/>
-    <mergeCell ref="B65:B68"/>
-    <mergeCell ref="C65:C68"/>
-    <mergeCell ref="D63:G64"/>
-    <mergeCell ref="D67:G68"/>
-    <mergeCell ref="D71:G72"/>
-    <mergeCell ref="A61:A64"/>
-    <mergeCell ref="B61:B64"/>
-    <mergeCell ref="C61:C64"/>
-    <mergeCell ref="H61:H64"/>
     <mergeCell ref="C39:C42"/>
     <mergeCell ref="H39:H42"/>
     <mergeCell ref="A43:A46"/>
     <mergeCell ref="B43:B46"/>
-    <mergeCell ref="C43:C46"/>
-    <mergeCell ref="H43:H46"/>
-    <mergeCell ref="A39:A42"/>
-    <mergeCell ref="G45:G46"/>
-    <mergeCell ref="F45:F46"/>
-    <mergeCell ref="E45:E46"/>
-    <mergeCell ref="D45:D46"/>
-    <mergeCell ref="H33:H35"/>
-    <mergeCell ref="A36:A38"/>
-    <mergeCell ref="B36:B38"/>
-    <mergeCell ref="C36:C38"/>
-    <mergeCell ref="H36:H38"/>
-    <mergeCell ref="A33:A35"/>
-    <mergeCell ref="B33:B35"/>
-    <mergeCell ref="C33:C35"/>
-    <mergeCell ref="H19:H23"/>
-    <mergeCell ref="A24:A26"/>
-    <mergeCell ref="B24:B26"/>
-    <mergeCell ref="C24:C26"/>
-    <mergeCell ref="A30:A32"/>
-    <mergeCell ref="B30:B32"/>
-    <mergeCell ref="C30:C32"/>
-    <mergeCell ref="H30:H32"/>
-    <mergeCell ref="H24:H26"/>
-    <mergeCell ref="D19:D20"/>
-    <mergeCell ref="E19:E20"/>
-    <mergeCell ref="F19:F20"/>
-    <mergeCell ref="G19:G20"/>
-    <mergeCell ref="G22:G23"/>
-    <mergeCell ref="F22:F23"/>
-    <mergeCell ref="E22:E23"/>
-    <mergeCell ref="H13:H15"/>
-    <mergeCell ref="A16:A18"/>
-    <mergeCell ref="B16:B18"/>
-    <mergeCell ref="C16:C18"/>
-    <mergeCell ref="H16:H18"/>
-    <mergeCell ref="G14:G15"/>
-    <mergeCell ref="F14:F15"/>
-    <mergeCell ref="E14:E15"/>
-    <mergeCell ref="H7:H9"/>
-    <mergeCell ref="A10:A12"/>
-    <mergeCell ref="B10:B12"/>
-    <mergeCell ref="C10:C12"/>
-    <mergeCell ref="D10:D12"/>
-    <mergeCell ref="E10:E12"/>
-    <mergeCell ref="F10:F12"/>
-    <mergeCell ref="G10:G12"/>
-    <mergeCell ref="H10:H12"/>
-    <mergeCell ref="G7:G9"/>
-    <mergeCell ref="A19:A23"/>
-    <mergeCell ref="B19:B23"/>
-    <mergeCell ref="C19:C23"/>
-    <mergeCell ref="A7:A9"/>
-    <mergeCell ref="B7:B9"/>
-    <mergeCell ref="C7:C9"/>
-    <mergeCell ref="D7:D9"/>
-    <mergeCell ref="E7:E9"/>
-    <mergeCell ref="F7:F9"/>
-    <mergeCell ref="A13:A15"/>
-    <mergeCell ref="B13:B15"/>
-    <mergeCell ref="C13:C15"/>
-    <mergeCell ref="D13:D15"/>
-    <mergeCell ref="D22:D23"/>
-    <mergeCell ref="H1:H3"/>
-    <mergeCell ref="H4:H6"/>
-    <mergeCell ref="E2:G2"/>
-    <mergeCell ref="D1:G1"/>
-    <mergeCell ref="G4:G6"/>
-    <mergeCell ref="A1:A3"/>
-    <mergeCell ref="D2:D3"/>
-    <mergeCell ref="C1:C3"/>
-    <mergeCell ref="B1:B3"/>
-    <mergeCell ref="F4:F6"/>
-    <mergeCell ref="E4:E6"/>
-    <mergeCell ref="D4:D6"/>
-    <mergeCell ref="C4:C6"/>
-    <mergeCell ref="B4:B6"/>
-    <mergeCell ref="A4:A6"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0" r:id="rId1"/>

</xml_diff>